<commit_message>
Add Set of Usecase.docx Add UC
</commit_message>
<xml_diff>
--- a/WIP/Users/MaiCTP/UC.xlsx
+++ b/WIP/Users/MaiCTP/UC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="144">
   <si>
     <t>NO.</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Search user's account</t>
   </si>
   <si>
-    <t>Export list users</t>
-  </si>
-  <si>
     <t>View(review) project</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Add new category</t>
   </si>
   <si>
-    <t>Edit category</t>
-  </si>
-  <si>
     <t>Export list categories</t>
   </si>
   <si>
@@ -318,12 +312,6 @@
     <t>UC38</t>
   </si>
   <si>
-    <t>View Timeline</t>
-  </si>
-  <si>
-    <t>View list public backer</t>
-  </si>
-  <si>
     <t>UC1</t>
   </si>
   <si>
@@ -375,71 +363,98 @@
     <t>Search backing</t>
   </si>
   <si>
-    <t>Export list backings</t>
+    <t>Preview slider</t>
+  </si>
+  <si>
+    <t>UC39</t>
+  </si>
+  <si>
+    <t>Manage Report</t>
+  </si>
+  <si>
+    <t>Change report's status</t>
+  </si>
+  <si>
+    <t>View report list</t>
+  </si>
+  <si>
+    <t>View report detail</t>
+  </si>
+  <si>
+    <t>UC40</t>
+  </si>
+  <si>
+    <t>UC41</t>
+  </si>
+  <si>
+    <t>View dashboard</t>
+  </si>
+  <si>
+    <t>UC42</t>
+  </si>
+  <si>
+    <t>UC43</t>
+  </si>
+  <si>
+    <t>UC44</t>
+  </si>
+  <si>
+    <t>Manage user's account</t>
+  </si>
+  <si>
+    <t>Manage projects</t>
+  </si>
+  <si>
+    <t>Manage backings</t>
+  </si>
+  <si>
+    <t>Manage Categories</t>
+  </si>
+  <si>
+    <t>Manage Sliders</t>
+  </si>
+  <si>
+    <t>Manage Message</t>
+  </si>
+  <si>
+    <t>View comments</t>
+  </si>
+  <si>
+    <t>View schedule</t>
+  </si>
+  <si>
+    <t>View Link Backers</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Export list users     x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export list backings       </t>
+  </si>
+  <si>
+    <t>Edit category       x</t>
   </si>
   <si>
     <t>View backing's information</t>
   </si>
   <si>
-    <t>Preview slider</t>
-  </si>
-  <si>
-    <t>UC39</t>
-  </si>
-  <si>
-    <t>Manage Report</t>
-  </si>
-  <si>
-    <t>Change report's status</t>
-  </si>
-  <si>
-    <t>View report list</t>
-  </si>
-  <si>
-    <t>View report detail</t>
-  </si>
-  <si>
-    <t>UC40</t>
-  </si>
-  <si>
-    <t>UC41</t>
-  </si>
-  <si>
-    <t>View dashboard</t>
-  </si>
-  <si>
-    <t>UC42</t>
-  </si>
-  <si>
-    <t>UC43</t>
-  </si>
-  <si>
-    <t>UC44</t>
-  </si>
-  <si>
-    <t>Manage user's account</t>
-  </si>
-  <si>
-    <t>Manage projects</t>
-  </si>
-  <si>
-    <t>Manage backings</t>
-  </si>
-  <si>
-    <t>Manage Categories</t>
-  </si>
-  <si>
-    <t>Manage Sliders</t>
-  </si>
-  <si>
-    <t>Manage Message</t>
+    <t xml:space="preserve">View message              </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>View dashboard   x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +481,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -594,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -622,45 +643,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,6 +663,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1003,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,14 +1037,14 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1033,416 +1055,541 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="34"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="22"/>
+      <c r="D7" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="34"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="22"/>
+      <c r="D8" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="34"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="22"/>
+      <c r="D9" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="22"/>
+      <c r="D10" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="34"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="35"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="D20" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="21"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="21"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="22"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="24"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="24"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="24"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="25"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="37"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="37"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="37"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="37"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="37"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="38"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>137</v>
+      <c r="C32" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="27"/>
+        <v>19</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="27"/>
+        <v>20</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="27"/>
+        <v>21</v>
+      </c>
+      <c r="C35" s="35"/>
+      <c r="D35" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="27"/>
+        <v>115</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C37" s="35"/>
+      <c r="D37" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="28"/>
+        <v>23</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>138</v>
+        <v>92</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="30"/>
+        <v>25</v>
+      </c>
+      <c r="C40" s="38"/>
+      <c r="D40" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="30"/>
+        <v>24</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="30"/>
+        <v>141</v>
+      </c>
+      <c r="C42" s="38"/>
+      <c r="D42" s="19" t="s">
+        <v>142</v>
+      </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="31"/>
+        <v>27</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="19"/>
+        <v>120</v>
+      </c>
+      <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="19"/>
+        <v>118</v>
+      </c>
+      <c r="C46" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1462,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,11 +1624,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1496,110 +1643,110 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>79</v>
+        <v>63</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="40"/>
+        <v>64</v>
+      </c>
+      <c r="C6" s="41"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="40"/>
+        <v>133</v>
+      </c>
+      <c r="C7" s="41"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="40"/>
+        <v>134</v>
+      </c>
+      <c r="C8" s="41"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>80</v>
-      </c>
+      <c r="A9" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="41"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="41"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="41"/>
+        <v>26</v>
+      </c>
+      <c r="C12" s="42"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="15"/>
+      <c r="A13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>68</v>
@@ -1608,198 +1755,207 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>112</v>
-      </c>
+      <c r="A17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="42"/>
+        <v>69</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="42"/>
+        <v>70</v>
+      </c>
+      <c r="C19" s="43"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="42"/>
+        <v>71</v>
+      </c>
+      <c r="C20" s="43"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="42"/>
+        <v>72</v>
+      </c>
+      <c r="C21" s="43"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="42"/>
+        <v>73</v>
+      </c>
+      <c r="C22" s="43"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="15"/>
+      <c r="A23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="43"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>85</v>
-      </c>
+      <c r="A28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="43"/>
+        <v>84</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="43"/>
+        <v>80</v>
+      </c>
+      <c r="C30" s="44"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="43"/>
+        <v>82</v>
+      </c>
+      <c r="C31" s="44"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>114</v>
-      </c>
+      <c r="A32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="44"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="39"/>
+        <v>87</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="39"/>
+        <v>86</v>
+      </c>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C33:C35"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="C29:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>